<commit_message>
Cambio Excel y matriz
</commit_message>
<xml_diff>
--- a/Bosque.xlsx
+++ b/Bosque.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karla\OneDrive - Instituto Politecnico Nacional\Desktop\Materias\Pattern Recognition\Proyecto1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonic\Documents\ESCOM\Octavo Semestre\Pattern Recognition\Pattern-Recognition-Proyecto-1-main-2\Pattern-Recognition-Proyecto-1-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF1D933-5597-42E2-9B67-C9F4F99D3A10}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159425F0-3B27-4680-84D8-384F1C6CDF68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{A85DA846-1181-4EBF-828E-2ACCBB65E1B7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A85DA846-1181-4EBF-828E-2ACCBB65E1B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -502,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D236C386-60C0-4B93-A8D7-4C88E4C4CCCF}">
-  <dimension ref="A1:P1807"/>
+  <dimension ref="A1:P1806"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1788" workbookViewId="0">
-      <selection activeCell="H1807" sqref="H1807"/>
+    <sheetView tabSelected="1" topLeftCell="A1791" workbookViewId="0">
+      <selection activeCell="K1808" sqref="K1808"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20530,6 +20530,21 @@
       <c r="C1800">
         <v>126</v>
       </c>
+      <c r="I1800" s="1">
+        <f>SUM(A2:A1806)</f>
+        <v>184309</v>
+      </c>
+      <c r="J1800" s="1">
+        <f>SUM(B2:B1806)</f>
+        <v>142831</v>
+      </c>
+      <c r="K1800" s="1">
+        <f>SUM(C2:C1806)</f>
+        <v>100754</v>
+      </c>
+      <c r="L1800" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="1801" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1801">
@@ -20541,20 +20556,17 @@
       <c r="C1801">
         <v>122</v>
       </c>
-      <c r="I1801" s="1">
-        <f>SUM(A2:A1806)</f>
-        <v>184309</v>
-      </c>
-      <c r="J1801" s="1">
-        <f>SUM(B2:B1806)</f>
-        <v>142831</v>
-      </c>
-      <c r="K1801" s="1">
-        <f>SUM(C2:C1806)</f>
-        <v>100754</v>
-      </c>
-      <c r="L1801" s="1" t="s">
-        <v>0</v>
+      <c r="I1801" s="2">
+        <v>102.11020000000001</v>
+      </c>
+      <c r="J1801" s="2">
+        <v>79.130700000000004</v>
+      </c>
+      <c r="K1801" s="2">
+        <v>55.819299999999998</v>
+      </c>
+      <c r="L1801" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="1802" spans="1:12" x14ac:dyDescent="0.25">
@@ -20567,18 +20579,6 @@
       <c r="C1802">
         <v>115</v>
       </c>
-      <c r="I1802" s="2">
-        <v>102.11020000000001</v>
-      </c>
-      <c r="J1802" s="2">
-        <v>79.130700000000004</v>
-      </c>
-      <c r="K1802" s="2">
-        <v>55.819299999999998</v>
-      </c>
-      <c r="L1802" s="2" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="1803" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1803">
@@ -20623,17 +20623,15 @@
       <c r="C1806">
         <v>115</v>
       </c>
-    </row>
-    <row r="1807" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E1807" s="3">
+      <c r="E1806" s="3">
         <f>AVERAGE(A2:A1806)</f>
         <v>102.11024930747922</v>
       </c>
-      <c r="F1807" s="3">
+      <c r="F1806" s="3">
         <f>AVERAGE(B2:B1806)</f>
         <v>79.130747922437678</v>
       </c>
-      <c r="G1807" s="3">
+      <c r="G1806" s="3">
         <f>AVERAGE(C2:C1806)</f>
         <v>55.81939058171745</v>
       </c>

</xml_diff>